<commit_message>
Sales JobChange Datetime add
</commit_message>
<xml_diff>
--- a/ImpTemplate/置业顾问模板.xlsx
+++ b/ImpTemplate/置业顾问模板.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t xml:space="preserve">电话 </t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -66,6 +66,34 @@
   <si>
     <t>2018-10-01</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>部门ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>部门名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>销售一部</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>销售二部</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>岗位类型</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>主管</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>员工</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -433,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -447,7 +475,7 @@
     <col min="4" max="4" width="12.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -460,8 +488,17 @@
       <c r="D1" t="s">
         <v>7</v>
       </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -471,8 +508,17 @@
       <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="E2">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -482,8 +528,17 @@
       <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -496,8 +551,17 @@
       <c r="D4" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -506,6 +570,15 @@
       </c>
       <c r="C5" s="2" t="s">
         <v>11</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>